<commit_message>
adding working files to Documents
</commit_message>
<xml_diff>
--- a/Documentation/AgileBacklogTemplate.xlsx
+++ b/Documentation/AgileBacklogTemplate.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>Conestoga College</t>
   </si>
@@ -99,6 +99,15 @@
   </si>
   <si>
     <t>JP, MD, RT, KW</t>
+  </si>
+  <si>
+    <t>Log In</t>
+  </si>
+  <si>
+    <t>wishlist / friends</t>
+  </si>
+  <si>
+    <t>Change Password</t>
   </si>
 </sst>
 </file>
@@ -129,7 +138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,6 +169,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -173,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -204,6 +219,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -510,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+      <selection activeCell="C28" sqref="C28:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,91 +702,132 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="2"/>
+      <c r="A18" s="14">
+        <v>15</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="16">
+        <v>6</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
+      <c r="B19" s="12"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
+      <c r="B20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="11" t="s">
+      <c r="A21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="10"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="11" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>3</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26">
-        <v>5</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>7</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27">
-        <v>5</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>7</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>10</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B30" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C28">
+      <c r="C30">
         <v>6</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="9" t="s">
+      <c r="D30" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="B31" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="s">
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="11" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="16">
+        <v>18</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="16">
+        <v>5</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="13"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated documents, event table, agilebacklog
</commit_message>
<xml_diff>
--- a/Documentation/AgileBacklogTemplate.xlsx
+++ b/Documentation/AgileBacklogTemplate.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="61">
   <si>
     <t>Conestoga College</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>By</t>
-  </si>
-  <si>
     <t>High Priority</t>
   </si>
   <si>
@@ -104,10 +101,109 @@
     <t>Log In</t>
   </si>
   <si>
-    <t>wishlist / friends</t>
-  </si>
-  <si>
     <t>Change Password</t>
+  </si>
+  <si>
+    <t>Resources</t>
+  </si>
+  <si>
+    <t>View profile</t>
+  </si>
+  <si>
+    <t>Edit profile</t>
+  </si>
+  <si>
+    <t>Edit mailing address</t>
+  </si>
+  <si>
+    <t>Edit shipping address</t>
+  </si>
+  <si>
+    <t>Search games</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check out </t>
+  </si>
+  <si>
+    <t>Submit order</t>
+  </si>
+  <si>
+    <t>View cart</t>
+  </si>
+  <si>
+    <t>Edit cart</t>
+  </si>
+  <si>
+    <t>Update status of ship</t>
+  </si>
+  <si>
+    <t>Remove game from wish list</t>
+  </si>
+  <si>
+    <t>View friend's wish list</t>
+  </si>
+  <si>
+    <t>Add game review</t>
+  </si>
+  <si>
+    <t>Download game</t>
+  </si>
+  <si>
+    <t>View pending shipments</t>
+  </si>
+  <si>
+    <t>View own wishlist</t>
+  </si>
+  <si>
+    <t>Reset password</t>
+  </si>
+  <si>
+    <t>Visitor registers</t>
+  </si>
+  <si>
+    <t>View game details</t>
+  </si>
+  <si>
+    <t>Add to cart</t>
+  </si>
+  <si>
+    <t>Delete from cart</t>
+  </si>
+  <si>
+    <t>Log out</t>
+  </si>
+  <si>
+    <t>Add credit card</t>
+  </si>
+  <si>
+    <t>View friends</t>
+  </si>
+  <si>
+    <t>Add friend</t>
+  </si>
+  <si>
+    <t>Delete friend</t>
+  </si>
+  <si>
+    <t>Publish review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete credit card </t>
+  </si>
+  <si>
+    <t>Add to wish list</t>
+  </si>
+  <si>
+    <t>Rate game</t>
+  </si>
+  <si>
+    <t>Register for event</t>
+  </si>
+  <si>
+    <t>View pending reviews</t>
+  </si>
+  <si>
+    <t>Reject review</t>
   </si>
 </sst>
 </file>
@@ -188,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -230,6 +326,25 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -535,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28:C30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,16 +669,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -582,17 +697,17 @@
         <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E7" s="10"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -600,7 +715,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -608,13 +723,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -622,13 +737,13 @@
         <v>2</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <v>7</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -636,13 +751,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13">
         <v>7</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -650,13 +765,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <v>7</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -664,13 +779,13 @@
         <v>6</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>7</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -678,156 +793,640 @@
         <v>8</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16">
         <v>7</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>9</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17">
         <v>4</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>15</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="16">
         <v>6</v>
       </c>
       <c r="D18" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="18">
+        <v>14</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="20">
+        <v>6</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18">
+        <v>16</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="20">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="21">
+        <v>19</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="20">
+        <v>6</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18">
+        <v>24</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="20">
+        <v>4</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="18">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="12"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="11" t="s">
+      <c r="B24" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="20">
+        <v>3</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18">
+        <v>34</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="20">
+        <v>4</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="18">
+        <v>35</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="20">
+        <v>4</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="18">
+        <v>36</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="20">
+        <v>4</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="21">
+        <v>37</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="20">
+        <v>4</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="18">
+        <v>40</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="20">
+        <v>4</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="21">
+        <v>45</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="20">
+        <v>4</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="21">
+        <v>46</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="20">
+        <v>5</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
+    </row>
+    <row r="33" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="18">
+        <v>22</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="20">
+        <v>4</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="18">
+        <v>28</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="20">
+        <v>4</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="18">
+        <v>29</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="20">
+        <v>4</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="18">
+        <v>30</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="20">
+        <v>3</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="18">
+        <v>38</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="20">
+        <v>4</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="21">
+        <v>43</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="20">
+        <v>3</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="23"/>
+      <c r="B39" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="7" t="s">
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="10"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>3</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>7</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42">
+        <v>5</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>10</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43">
+        <v>6</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="13"/>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="21">
+        <v>17</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" s="20">
+        <v>5</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="21">
+        <v>20</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" s="20">
+        <v>4</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="21">
+        <v>21</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" s="20">
+        <v>4</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="13"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="18">
+        <v>11</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51" s="20">
+        <v>4</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="18">
+        <v>13</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" s="20">
+        <v>4</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="18">
+        <v>23</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" s="20">
+        <v>3</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="18">
+        <v>26</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54" s="20">
+        <v>4</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="18">
+        <v>27</v>
+      </c>
+      <c r="B55" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C55" s="20">
+        <v>4</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="18">
+        <v>32</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" s="20">
+        <v>4</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="18">
+        <v>33</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C57" s="20">
+        <v>5</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="18">
+        <v>39</v>
+      </c>
+      <c r="B58" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58" s="20">
+        <v>4</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="21">
+        <v>41</v>
+      </c>
+      <c r="B59" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C59" s="20">
+        <v>3</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="21">
+        <v>42</v>
+      </c>
+      <c r="B60" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C60" s="20">
+        <v>3</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="21">
+        <v>44</v>
+      </c>
+      <c r="B61" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61" s="20">
+        <v>3</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="24"/>
+      <c r="B62" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="10"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="11" t="s">
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="B63" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="14">
+        <v>18</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C64" s="16">
+        <v>5</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+      <c r="B65" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>3</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28">
-        <v>5</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+      <c r="B67" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29">
-        <v>5</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>10</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30">
-        <v>6</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="16">
-        <v>18</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="16">
-        <v>5</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="13"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="13" t="s">
-        <v>27</v>
+    </row>
+    <row r="68" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="18">
+        <v>31</v>
+      </c>
+      <c r="B68" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C68" s="20">
+        <v>4</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated RT Individual Status Report
</commit_message>
<xml_diff>
--- a/Documentation/AgileBacklogTemplate.xlsx
+++ b/Documentation/AgileBacklogTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PROG3050\Project\Git\Grey-Cube-Development\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Level5\MSEnterprise\Grey-Cube-Development\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -652,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:XFD66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,20 +1386,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="14">
-        <v>18</v>
-      </c>
-      <c r="B64" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C64" s="16">
-        <v>5</v>
-      </c>
-      <c r="D64" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="11" t="s">
@@ -1407,7 +1393,18 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
+      <c r="A66" s="14">
+        <v>18</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66" s="16">
+        <v>5</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>

</xml_diff>